<commit_message>
new parsers has been added
</commit_message>
<xml_diff>
--- a/topovi_products.xlsx
+++ b/topovi_products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K402"/>
+  <dimension ref="A1:K454"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20920,6 +20920,2800 @@
         </is>
       </c>
     </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>Anima Beige Fullbody 3D</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>Anima Beige Fullbody 3D</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Anima-Beige-Fullbody-3D1.webp</t>
+        </is>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Anima-Beige-Fullbody-3D1.webp</t>
+        </is>
+      </c>
+      <c r="H403" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Anima%20Beige%20Fullbody%203d-int.webp</t>
+        </is>
+      </c>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Anima-Beige-Fullbody-3D2.webp</t>
+        </is>
+      </c>
+      <c r="J403" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Anima-Beige-Fullbody-3D3.webp</t>
+        </is>
+      </c>
+      <c r="K403" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Anima-Beige-Fullbody-3D4.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>Arabescato Viola</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>Arabescato Viola</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Arabescato-Viola-%D0%901.webp</t>
+        </is>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>Глянець</t>
+        </is>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Arabescato-Viola-%D0%901.webp</t>
+        </is>
+      </c>
+      <c r="H404" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Arabescato-Viola-%D0%92.webp</t>
+        </is>
+      </c>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Arabescato-Viola42.webp</t>
+        </is>
+      </c>
+      <c r="J404" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Arabescato-Viola4.webp</t>
+        </is>
+      </c>
+      <c r="K404" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Arabescato-Viola2.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>Aurora Black</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>Aurora Black</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Aurora-Black1.webp</t>
+        </is>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>Структурована</t>
+        </is>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Aurora-Black1.webp</t>
+        </is>
+      </c>
+      <c r="H405" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Aurora-Black-5.webp</t>
+        </is>
+      </c>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Aurora-Black-3.webp</t>
+        </is>
+      </c>
+      <c r="J405" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Aurora-Black-6.webp</t>
+        </is>
+      </c>
+      <c r="K405" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Aurora-Black-2.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>Blue Stone Negro</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>Blue Stone Negro</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Blue-Stone-Negro1.webp</t>
+        </is>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G406" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Blue-Stone-Negro1.webp</t>
+        </is>
+      </c>
+      <c r="H406" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Blue-Stone-Negro-2.webp</t>
+        </is>
+      </c>
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Blue-Stone-Negro-3.webp</t>
+        </is>
+      </c>
+      <c r="J406" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Blue-Stone-Negro-5.webp</t>
+        </is>
+      </c>
+      <c r="K406" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Blue-Stone-Negro-56.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>Camargue Arena</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>Camargue Arena</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Camargue-Arena1.webp</t>
+        </is>
+      </c>
+      <c r="F407" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G407" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Camargue-Arena1.webp</t>
+        </is>
+      </c>
+      <c r="H407" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Camargue-Arena2.webp</t>
+        </is>
+      </c>
+      <c r="I407" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Camargue-Arena3.webp</t>
+        </is>
+      </c>
+      <c r="J407" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Camargue-Arena4.webp</t>
+        </is>
+      </c>
+      <c r="K407" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Camargue-Aren%D0%B05.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>Ceppo Di Gre Fullbody 3D</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>Ceppo Di Gre Fullbody 3D</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Ceppo-Di-Gre-Fullbody-3D1.webp</t>
+        </is>
+      </c>
+      <c r="F408" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G408" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Ceppo-Di-Gre-Fullbody-3D1.webp</t>
+        </is>
+      </c>
+      <c r="H408" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Ceppo-Di-Gre-Fullbody-3D-2.webp</t>
+        </is>
+      </c>
+      <c r="I408" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Ceppo-Di-Gre-Fullbody-3D-3.webp</t>
+        </is>
+      </c>
+      <c r="J408" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Ceppo-Di-Gre-Fullbody-3D-4.webp</t>
+        </is>
+      </c>
+      <c r="K408" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Ceppo-Di-Gre-Fullbody-3D-5.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>Distrito Marfil</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>Distrito Marfil</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Distrito-Marfil1.webp</t>
+        </is>
+      </c>
+      <c r="F409" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G409" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Distrito-Marfil1.webp</t>
+        </is>
+      </c>
+      <c r="H409" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Distrito-Marfil-3.webp</t>
+        </is>
+      </c>
+      <c r="I409" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Distrito-Marfil-4.webp</t>
+        </is>
+      </c>
+      <c r="J409" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Distrito-Marfil-5.webp</t>
+        </is>
+      </c>
+      <c r="K409" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Distrito-Marfil-6.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>Grey Soap Fullbody 3D</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>Grey Soap Fullbody 3D</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Grey-Soap-Fullbody-3D1.webp</t>
+        </is>
+      </c>
+      <c r="F410" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G410" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Grey-Soap-Fullbody-3D1.webp</t>
+        </is>
+      </c>
+      <c r="H410" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Grey-Soap-Fullbody-3D-1.webp</t>
+        </is>
+      </c>
+      <c r="I410" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Grey-Soap-Fullbody-3D-2.webp</t>
+        </is>
+      </c>
+      <c r="J410" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Grey-Soap-Fullbody-3D-3.webp</t>
+        </is>
+      </c>
+      <c r="K410" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Grey-Soap-Fullbody-3D-4.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>Light Red Calacatta</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>Light Red Calacatta</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Light-Red-Calacatta1.webp</t>
+        </is>
+      </c>
+      <c r="F411" t="inlineStr">
+        <is>
+          <t>Глянець</t>
+        </is>
+      </c>
+      <c r="G411" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Light-Red-Calacatta1.webp</t>
+        </is>
+      </c>
+      <c r="H411" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Light-Red-Calacatta-%D0%92.webp</t>
+        </is>
+      </c>
+      <c r="I411" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Light-Red-Calacatta2.webp</t>
+        </is>
+      </c>
+      <c r="J411" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Light-Red-Calacatta3.webp</t>
+        </is>
+      </c>
+      <c r="K411" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Light-Red-Calacatta4.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>Makrana</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>Makrana</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Makrana/Makrana_1.webp</t>
+        </is>
+      </c>
+      <c r="F412" t="inlineStr">
+        <is>
+          <t>Глянець</t>
+        </is>
+      </c>
+      <c r="G412" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Makrana/Makrana_1.webp</t>
+        </is>
+      </c>
+      <c r="H412" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Makrana/Makrana-2.webp</t>
+        </is>
+      </c>
+      <c r="I412" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Makrana/Makrana-3.webp</t>
+        </is>
+      </c>
+      <c r="J412" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Makrana/Makrana-4.webp</t>
+        </is>
+      </c>
+      <c r="K412" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Makrana/Makrana-5.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>Negev</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>Negev</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Negev-%D0%901.webp</t>
+        </is>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
+          <t>Глянець</t>
+        </is>
+      </c>
+      <c r="G413" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Negev-%D0%901.webp</t>
+        </is>
+      </c>
+      <c r="H413" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Negev-%D0%92.webp</t>
+        </is>
+      </c>
+      <c r="I413" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Negev2.webp</t>
+        </is>
+      </c>
+      <c r="J413" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Negev3.webp</t>
+        </is>
+      </c>
+      <c r="K413" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Negev4.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>Noir Laurent</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>Noir Laurent</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Noir-Laurent1.webp</t>
+        </is>
+      </c>
+      <c r="F414" t="inlineStr">
+        <is>
+          <t>Глянець</t>
+        </is>
+      </c>
+      <c r="G414" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Noir-Laurent1.webp</t>
+        </is>
+      </c>
+      <c r="H414" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Noir-Laurent-1.webp</t>
+        </is>
+      </c>
+      <c r="I414" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Noir-Laurent-2.webp</t>
+        </is>
+      </c>
+      <c r="J414" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Noir-Laurent-3.webp</t>
+        </is>
+      </c>
+      <c r="K414" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Noir-Laurent-4.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>Norwegian Stone Grey</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>Norwegian Stone Grey</t>
+        </is>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Norwegian-Stone-Grey1.webp</t>
+        </is>
+      </c>
+      <c r="F415" t="inlineStr">
+        <is>
+          <t>Структурована</t>
+        </is>
+      </c>
+      <c r="G415" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Norwegian-Stone-Grey1.webp</t>
+        </is>
+      </c>
+      <c r="H415" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Norwegian-Stone-Grey2.webp</t>
+        </is>
+      </c>
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Norwegian-Stone-Grey3.webp</t>
+        </is>
+      </c>
+      <c r="J415" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Norwegian-Stone-Grey4.webp</t>
+        </is>
+      </c>
+      <c r="K415" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Norwegian-Stone-Grey5.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>Pulpis Ivory</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>Pulpis Ivory</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Pulpis-Ivory1.webp</t>
+        </is>
+      </c>
+      <c r="F416" t="inlineStr">
+        <is>
+          <t>Глянець</t>
+        </is>
+      </c>
+      <c r="G416" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Pulpis-Ivory1.webp</t>
+        </is>
+      </c>
+      <c r="H416" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Pulpis-Ivory2.webp</t>
+        </is>
+      </c>
+      <c r="I416" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Pulpis-Ivory3.webp</t>
+        </is>
+      </c>
+      <c r="J416" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Pulpis-Ivory4.webp</t>
+        </is>
+      </c>
+      <c r="K416" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Pulpis-Ivory5.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>Travertino Stone Beige</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>Travertino Stone Beige</t>
+        </is>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Travertino-Stone-Beige1.webp</t>
+        </is>
+      </c>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>Структурована</t>
+        </is>
+      </c>
+      <c r="G417" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Travertino-Stone-Beige1.webp</t>
+        </is>
+      </c>
+      <c r="H417" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Travertino-Stone-Beige2.webp</t>
+        </is>
+      </c>
+      <c r="I417" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Travertino-Stone-Beige3.webp</t>
+        </is>
+      </c>
+      <c r="J417" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Travertino-Stone-Beige4.webp</t>
+        </is>
+      </c>
+      <c r="K417" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Travertino-Stone-Beige5.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>Pietra Grigia</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>Pietra Grigia</t>
+        </is>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/Pietra%20Grigia%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F418" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G418" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Pietra%20Grigia%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H418" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Pietra-Grigia-Natural%201.webp</t>
+        </is>
+      </c>
+      <c r="I418" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Pietra-Grigia-Natural-2.webp</t>
+        </is>
+      </c>
+      <c r="J418" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Pietra-Grigia-Natural.webp</t>
+        </is>
+      </c>
+      <c r="K418" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Pietra%20Grigia/Pietra_Grigia_A_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>Boulevard Grey</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>Boulevard Grey</t>
+        </is>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Boulevard%20Grey/Boulevard_Grey_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F419" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G419" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Boulevard%20Grey/Boulevard_Grey_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H419" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Boulevard%20Grey/Boulevard_Grey_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I419" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Boulevard%20Grey/Boulevard_Grey_sl1_v2.webp</t>
+        </is>
+      </c>
+      <c r="J419" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Boulevard%20Grey/Boulevard_Grey_sl2_v2.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>Calacatta Gold Bookmatch A-B</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>Calacatta Gold Bookmatch A-B</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Calacatta%20gold%20bookmatch%20a-b%20natural/Infinito%202.0%20Calacatta%20Gold%20Honed%20Bookmatch%20A-B_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F420" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G420" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20gold%20bookmatch%20a-b%20natural/Infinito%202.0%20Calacatta%20Gold%20Honed%20Bookmatch%20A-B_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H420" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20gold%20bookmatch%20a-b%20natural/Infinito%202.0%20Calacatta%20Gold%20Honed%20Bookmatch%20A-%20B_1.webp</t>
+        </is>
+      </c>
+      <c r="I420" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20gold%20bookmatch%20a-b%20natural/Infinito%202.0%20Calacatta%20Gold%20Honed%20Bookmatch%20A-B_slab.webp</t>
+        </is>
+      </c>
+      <c r="J420" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20gold%20bookmatch%20a-b%20natural/Infinito%202.0%20Calacatta%20Gold%20Honed%20Bookmatch%20A-%20B_3.webp</t>
+        </is>
+      </c>
+      <c r="K420" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20gold%20bookmatch%20a-b%20natural/Infinito%202.0%20Calacatta%20Gold%20Honed%20Bookmatch%20A-%20B_2.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>Carrara C</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>Carrara C</t>
+        </is>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Infinito%202.0%20Carrara%20C%20Honed_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F421" t="inlineStr">
+        <is>
+          <t>Напівматова</t>
+        </is>
+      </c>
+      <c r="G421" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Carrara%20C%20Honed_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H421" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Carrara%20C%20Honed.webp</t>
+        </is>
+      </c>
+      <c r="I421" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Carrara%20C%20Honed_1.webp</t>
+        </is>
+      </c>
+      <c r="J421" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Carrara%20C%20Honed_2.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>Fior Di Bosco Honed</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>Fior Di Bosco Honed</t>
+        </is>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Fior%20di%20bosco%20honed/Infinito%202.0%20Fior%20Di%20Bosco%20Honed_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F422" t="inlineStr">
+        <is>
+          <t>Напівматова</t>
+        </is>
+      </c>
+      <c r="G422" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20di%20bosco%20honed/Infinito%202.0%20Fior%20Di%20Bosco%20Honed_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H422" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20di%20bosco%20honed/Infinito%202.0%20Fior%20Di%20Bosco%20Honed_1.webp</t>
+        </is>
+      </c>
+      <c r="I422" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20di%20bosco%20honed/Infinito%202.0%20Fior%20Di%20Bosco%20Honed_2.webp</t>
+        </is>
+      </c>
+      <c r="J422" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20di%20bosco%20honed/Infinito%202.0%20Fior%20Di%20Bosco%20Honed_3.webp</t>
+        </is>
+      </c>
+      <c r="K422" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20di%20bosco%20honed/Infinito%202.0%20Fior%20Di%20Bosco%20Honed_4.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>Lincoln</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>Lincoln</t>
+        </is>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Infinito%202.0%20Lincoln%20Polished_ZOOM_.webp</t>
+        </is>
+      </c>
+      <c r="F423" t="inlineStr">
+        <is>
+          <t>Глянець</t>
+        </is>
+      </c>
+      <c r="G423" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Lincoln%20Polished_ZOOM_.webp</t>
+        </is>
+      </c>
+      <c r="H423" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Lincoln%20Polished.webp</t>
+        </is>
+      </c>
+      <c r="I423" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Lincoln%20Polished_int1.webp</t>
+        </is>
+      </c>
+      <c r="J423" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Lincoln%20Polished_int2.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>Ombra di Caravaggio</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>Ombra di Caravaggio</t>
+        </is>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Infinito%202.0%20Ombra%20Di%20Caravaggio%20Glossy_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F424" t="inlineStr">
+        <is>
+          <t>Напівматова</t>
+        </is>
+      </c>
+      <c r="G424" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Ombra%20Di%20Caravaggio%20Glossy_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H424" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Ombra%20Di%20Caravaggio%20Glossy.webp</t>
+        </is>
+      </c>
+      <c r="I424" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Ombra%20Di%20Caravaggio%20Glossy_1.webp</t>
+        </is>
+      </c>
+      <c r="J424" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Ombra%20Di%20Caravaggio%20Glossy_2.webp</t>
+        </is>
+      </c>
+      <c r="K424" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Infinito%202.0%20Ombra%20Di%20Caravaggio%20Glossy_3.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>Statuario Extra Bookmatch A-B</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>Statuario Extra Bookmatch A-B</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Statuario%20extra%20bookmatch%20a-b%20natural/Infinito%202.0%20Statuario%20Extra%20Honed%20Bookmatch%20A-B_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G425" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20extra%20bookmatch%20a-b%20natural/Infinito%202.0%20Statuario%20Extra%20Honed%20Bookmatch%20A-B_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H425" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20extra%20bookmatch%20a-b%20natural/Infinito%202.0%20Statuario%20Extra%20Honed%20Bookmatch%20A-B_1.webp</t>
+        </is>
+      </c>
+      <c r="I425" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20extra%20bookmatch%20a-b%20natural/Infinito%202.0%20Statuario%20Extra%20Honed%20Bookmatch%20A-B_2.webp</t>
+        </is>
+      </c>
+      <c r="J425" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20extra%20bookmatch%20a-b%20natural/Infinito%202.0%20Statuario%20Extra%20Honed%20Bookmatch%20A-B_3.webp</t>
+        </is>
+      </c>
+      <c r="K425" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20extra%20bookmatch%20a-b%20natural/Infinito%202.0%20Statuario%20Extra%20Honed%20Bookmatch%20A-B_slab.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>Cement Ash</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>Cement Ash</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/Cement%20Ash%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G426" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Cement%20Ash%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H426" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Cement%20Ash%20Matt.webp</t>
+        </is>
+      </c>
+      <c r="I426" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Cement-Ash-Natural%201.webp</t>
+        </is>
+      </c>
+      <c r="J426" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Cement-Ash-Natural-2.webp</t>
+        </is>
+      </c>
+      <c r="K426" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Cement-Ash-Natural.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>Epiphany</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>Epiphany</t>
+        </is>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/Epiphany%20Polished_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>Глянець</t>
+        </is>
+      </c>
+      <c r="G427" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Epiphany%20Polished_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H427" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Epiphany%20Polished.webp</t>
+        </is>
+      </c>
+      <c r="I427" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Epiphany%20Polished_INT.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>Madera</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>Madera</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/Madera%20Matt_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Madera%20Matt_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H428" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Madera%20Matt_slab.webp</t>
+        </is>
+      </c>
+      <c r="I428" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Madera%20Matt_int.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>Pierre Bleu</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>Pierre Bleu</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/Pierre%20Bleu%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G429" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Pierre%20Bleu%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H429" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Pierre%20Bleu%20Matt.webp</t>
+        </is>
+      </c>
+      <c r="I429" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Pierre%20Bleu%20Matt_INT.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>Absolute</t>
+        </is>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Absolute/Absolute_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Absolute/Absolute_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H430" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Absolute/Absolute_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I430" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Absolute/Absolute_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J430" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Absolute/Absolute_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>Arabescato</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>Arabescato</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Arabescato/Arabescato_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G431" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Arabescato/Arabescato_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H431" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Arabescato/Arabescato_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I431" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Arabescato/Arabescato_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J431" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Arabescato/Arabescato_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>Black Diamond</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>Black Diamond</t>
+        </is>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Black%20Diamond/Black_Diamond_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G432" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Black%20Diamond/Black_Diamond_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H432" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Black%20Diamond/Black_Diamond_int.webp</t>
+        </is>
+      </c>
+      <c r="I432" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Black%20Diamond/Black_Diamond_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J432" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Black%20Diamond/Black_Diamond_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>Boulevard Black</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>Boulevard Black</t>
+        </is>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Boulevard%20Black/Boulevard_Black_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G433" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Boulevard%20Black/Boulevard_Black_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H433" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Boulevard%20Black/Boulevard_Black_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I433" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Boulevard%20Black/Boulevard_Black_sl1_v2.webp</t>
+        </is>
+      </c>
+      <c r="J433" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Boulevard%20Black/Boulevard_Black_sl2_v2.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>Calacatta Dorato</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>Calacatta Dorato</t>
+        </is>
+      </c>
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/Calacatta-Dorato1.webp</t>
+        </is>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G434" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Calacatta-Dorato1.webp</t>
+        </is>
+      </c>
+      <c r="H434" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Calacatta-Dorato-%D0%92.webp</t>
+        </is>
+      </c>
+      <c r="I434" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Calacatta-Dorato3.webp</t>
+        </is>
+      </c>
+      <c r="J434" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Calacatta-Dorato4.webp</t>
+        </is>
+      </c>
+      <c r="K434" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/Calacatta-Dorato5.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>Calacatta Oro</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>Calacatta Oro</t>
+        </is>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Calacatta%20Oro/Calacatta_Oro_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G435" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20Oro/Calacatta_Oro_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H435" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20Oro/Calacatta_Oro_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I435" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20Oro/Calacatta_Oro_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J435" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Calacatta%20Oro/Calacatta_Oro_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>Fior di Bosco</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>Fior di Bosco</t>
+        </is>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Fior%20Di%20Bosco/Fior_di_Bosco_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20Di%20Bosco/Fior_di_Bosco_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H436" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20Di%20Bosco/Fior_di_Bosco_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I436" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20Di%20Bosco/Fior_di_Bosco_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J436" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Fior%20Di%20Bosco/Fior_di_Bosco_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>Hermon</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>Hermon</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Hermon/Hermon_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Hermon/Hermon_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H437" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Hermon/Hermon_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I437" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Hermon/Hermon_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J437" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Hermon/Hermon_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>Lasa White</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>Lasa White</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Lasa%20White/Lasa_White_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Lasa%20White/Lasa_White_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Lasa%20White/Lasa_White_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I438" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Lasa%20White/Lasa_White_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J438" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Lasa%20White/Lasa_White_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>Meraki</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>Meraki</t>
+        </is>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Meraki/Meraki_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G439" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Meraki/Meraki_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H439" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Meraki/Meraki_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I439" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Meraki/Meraki_A_sl_v3.webp</t>
+        </is>
+      </c>
+      <c r="J439" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Meraki/Meraki_B_sl_v3.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>Monte Bianco</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>Monte Bianco</t>
+        </is>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Monte%20Bianco/Monte_Bianco_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G440" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Monte%20Bianco/Monte_Bianco_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H440" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Monte%20Bianco/Monte_Bianco_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I440" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Monte%20Bianco/Monte_Bianco_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J440" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Monte%20Bianco/Monte_Bianco_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>Patagonia</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>Patagonia</t>
+        </is>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Patagonia/Patagonia_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G441" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Patagonia/Patagonia_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H441" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Patagonia/Patagonia_int.webp</t>
+        </is>
+      </c>
+      <c r="I441" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Patagonia/Patagonia_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J441" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Patagonia/Patagonia_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>Pietra Brown</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>Pietra Brown</t>
+        </is>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Pietra%20Brown/Pietra_Brown_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G442" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Pietra%20Brown/Pietra_Brown_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H442" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Pietra%20Brown/Pietra_Brown_int.webp</t>
+        </is>
+      </c>
+      <c r="I442" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Pietra%20Brown/Pietra_Brown_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J442" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Pietra%20Brown/Pietra_Brown_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>Statuario Leonardo</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>Statuario Leonardo</t>
+        </is>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Statuario%20Leonardo/Statuario_Leonardo_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20Leonardo/Statuario_Leonardo_zoom_v2.webp</t>
+        </is>
+      </c>
+      <c r="H443" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20Leonardo/Statuario_Leonardo_int_v2.webp</t>
+        </is>
+      </c>
+      <c r="I443" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20Leonardo/Statuario_Leonardo_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J443" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20Leonardo/Statuario_Leonardo_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>Statuario Raffaello</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>Statuario Raffaello</t>
+        </is>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Statuario%20Raffaello/Statuario_Raffaello_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G444" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20Raffaello/Statuario_Raffaello_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H444" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20Raffaello/Statuario_Raffaello_int.webp</t>
+        </is>
+      </c>
+      <c r="I444" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20Raffaello/Statuario_Raffaello_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J444" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Statuario%20Raffaello/Statuario_Raffaello_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>Tinta Unita Bianco</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>Tinta Unita Bianco</t>
+        </is>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Tinta%20Unita%20Bianco/Tinta_Unita_Bianco_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G445" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Tinta%20Unita%20Bianco/Tinta_Unita_Bianco_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H445" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Tinta%20Unita%20Bianco/Tinta_Unita_Bianco_INT.webp</t>
+        </is>
+      </c>
+      <c r="I445" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Tinta%20Unita%20Bianco/Tinta_Unita_Bianco_R.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>Tinta Unita Nero</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>Tinta Unita Nero</t>
+        </is>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Tinta%20Unita%20Nero/Tinta_Unita_Nero_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Tinta%20Unita%20Nero/Tinta_Unita_Nero_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H446" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Tinta%20Unita%20Nero/Tinta_Unita_Nero_INT.webp</t>
+        </is>
+      </c>
+      <c r="I446" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Tinta%20Unita%20Nero/Tinta_Unita_Nero_R.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>Travertino White</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>Travertino White</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Travertino%20White/Travertino_White_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Travertino%20White/Travertino_White_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H447" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Travertino%20White/Travertino_White_int.webp</t>
+        </is>
+      </c>
+      <c r="I447" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Travertino%20White/Travertino_White_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J447" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Travertino%20White/Travertino_White_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>Ballet</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>Ballet</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Ballet/Ballet_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Ballet/Ballet_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H448" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Ballet/Ballet_INT.webp</t>
+        </is>
+      </c>
+      <c r="I448" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Ballet/Ballet_A_sl_.webp</t>
+        </is>
+      </c>
+      <c r="J448" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Ballet/Ballet_B_sl_.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>Concrete Ash</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>Concrete Ash</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/Concrete%20Ash%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Concrete%20Ash%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H449" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Concrete%20Ash%20Matt.webp</t>
+        </is>
+      </c>
+      <c r="I449" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Concrete%20Ash%20Matt_INT.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>Kenya</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>Kenya</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/NC-Kenya-Natural_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Kenya-Natural_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H450" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Kenya-Natural%201.webp</t>
+        </is>
+      </c>
+      <c r="I450" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/NC-Kenya-Natural-2.webp</t>
+        </is>
+      </c>
+      <c r="J450" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Kenya/Kenya__A_sl.webp</t>
+        </is>
+      </c>
+      <c r="K450" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Kenya/Kenya__B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>Marmo Antico</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>Marmo Antico</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Marmo%20Antico%20Natural/NC_Marmo_Antico_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Marmo%20Antico%20Natural/NC_Marmo_Antico_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H451" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Marmo%20Antico%20Natural/NC_Marmo_Antico_int.webp</t>
+        </is>
+      </c>
+      <c r="I451" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Marmo%20Antico%20Natural/Marmo_Antico__A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J451" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Marmo%20Antico%20Natural/Marmo_Antico__B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>Nero Marquina</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>Nero Marquina</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/Nero%20Marquina%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Nero%20Marquina%20Matt_ZOOM.webp</t>
+        </is>
+      </c>
+      <c r="H452" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nero%20Marquina%20Matt_int.webp</t>
+        </is>
+      </c>
+      <c r="I452" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nero%20Marquina/Nero_Marquina_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J452" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nero%20Marquina/Nero_Marquina_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>Portoro</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>Portoro</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Nuovo%20Corso/Portoro%20Matt_zoom.webp</t>
+        </is>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Portoro%20Matt_zoom.webp</t>
+        </is>
+      </c>
+      <c r="H453" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Nuovo%20Corso/Portoro%20Matt_int.webp</t>
+        </is>
+      </c>
+      <c r="I453" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Portoro/Portoro_A_sl.webp</t>
+        </is>
+      </c>
+      <c r="J453" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Portoro/Portoro_B_sl.webp</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>Keralini</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Керамограніт</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>Taj Mahal</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>Taj Mahal</t>
+        </is>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/540/stones/keralini/Taj%20Mahal/Taj-Mahal.webp</t>
+        </is>
+      </c>
+      <c r="F454" t="inlineStr">
+        <is>
+          <t>Матова</t>
+        </is>
+      </c>
+      <c r="G454" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Taj%20Mahal/Taj-Mahal.webp</t>
+        </is>
+      </c>
+      <c r="H454" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Taj%20Mahal/Taj-Mahal1.webp</t>
+        </is>
+      </c>
+      <c r="I454" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Taj%20Mahal/Taj-Mahal2.webp</t>
+        </is>
+      </c>
+      <c r="J454" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Taj%20Mahal/Taj-Mahal3.webp</t>
+        </is>
+      </c>
+      <c r="K454" t="inlineStr">
+        <is>
+          <t>https://topovi.com.ua/media/images/1280/stones/keralini/Taj%20Mahal/Taj-Mahal4.webp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>